<commit_message>
Ajustes en plantilla de generacion de codigo
</commit_message>
<xml_diff>
--- a/Otros (Plantillas, etc)/plantilla codigo.xlsx
+++ b/Otros (Plantillas, etc)/plantilla codigo.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Generador Parametros" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparador Parametros" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
   <si>
     <t>IN PARAM_CCMPN</t>
   </si>
@@ -39,155 +39,272 @@
     <t>NUMERIC (10, 0),</t>
   </si>
   <si>
-    <t>IN PARAM_NITEM</t>
-  </si>
-  <si>
-    <t>NUMERIC (5,0),</t>
-  </si>
-  <si>
-    <t>IN PARAM_CDPRDC</t>
-  </si>
-  <si>
     <t>CHAR (10),</t>
   </si>
   <si>
-    <t>IN PARAM_SINSPR</t>
-  </si>
-  <si>
     <t>IN PARAM_SCNINP</t>
   </si>
   <si>
-    <t>IN PARAM_CFMLPR</t>
-  </si>
-  <si>
-    <t>IN PARAM_NTRMCR</t>
-  </si>
-  <si>
     <t>IN PARAM_SESTRG</t>
   </si>
   <si>
-    <t>IN PARAM_NSRIE1</t>
-  </si>
-  <si>
     <t>NUMERIC (6,0),</t>
   </si>
   <si>
-    <t>IN PARAM_NDCMSS</t>
-  </si>
-  <si>
-    <t>IN PARAM_STPCNS</t>
-  </si>
-  <si>
     <t>CHAR (1) ,</t>
   </si>
   <si>
-    <t>IN PARAM_UNIDAD</t>
-  </si>
-  <si>
-    <t>CHAR (2)</t>
-  </si>
-  <si>
-    <t>CHAR (1)</t>
-  </si>
-  <si>
-    <t>NUMERIC (3,0)</t>
-  </si>
-  <si>
-    <t>NUMERIC (10, 0)</t>
-  </si>
-  <si>
-    <t>NUMERIC (6,0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAR (1) </t>
-  </si>
-  <si>
-    <t>NUMERIC(8,0)</t>
-  </si>
-  <si>
-    <t>CHAR (10)</t>
-  </si>
-  <si>
     <t>IN PARAM_FCHCRT</t>
   </si>
   <si>
     <t>IN PARAM_HRACRT</t>
   </si>
   <si>
-    <t>IN PARAM_CUSCRT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN PARAM_IVUNIT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN PARAM_IVTOIT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN PARAM_CANTIDAD </t>
-  </si>
-  <si>
-    <t>NUMERIC (5,0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAR (2) </t>
-  </si>
-  <si>
-    <t>CHAR  (10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMERIC (6,0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMERIC (10,0) </t>
-  </si>
-  <si>
-    <t>NUMERIC ( 15, 5 )</t>
-  </si>
-  <si>
-    <t>NUMERIC ( 15,5 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMERIC (15,5) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAR (3) </t>
-  </si>
-  <si>
     <t>IN PARAM_CULUSA</t>
   </si>
   <si>
-    <t>NUMERIC (8,0),</t>
-  </si>
-  <si>
-    <t>IN PARAM_STPENT</t>
-  </si>
-  <si>
-    <t>IN PARAM_CENTD</t>
-  </si>
-  <si>
-    <t>IN PARAM_CRPRS</t>
-  </si>
-  <si>
-    <t>CHAR (5),</t>
-  </si>
-  <si>
-    <t>IN PARAM_NOPRCN</t>
-  </si>
-  <si>
-    <t>IN PARAM_SFRMRP</t>
-  </si>
-  <si>
-    <t>IN PARAM_FFRMRP</t>
-  </si>
-  <si>
-    <t>IN PARAM_HFRMRP</t>
+    <t>IN PARAM_NSLCPR</t>
+  </si>
+  <si>
+    <t>IN PARAM_USRCRT</t>
+  </si>
+  <si>
+    <t>CHAR  (10),</t>
+  </si>
+  <si>
+    <t>IN PARAM_NTRMNL</t>
+  </si>
+  <si>
+    <t>IN PARAM_CCLNT</t>
+  </si>
+  <si>
+    <t>NUMERIC (4,0),</t>
+  </si>
+  <si>
+    <t>NUMERIC (3,0),</t>
+  </si>
+  <si>
+    <t>IN PARAM_CTOPRC</t>
+  </si>
+  <si>
+    <t>IN PARAM_CTPOAL</t>
+  </si>
+  <si>
+    <t>NUMERIC (6, 0),</t>
+  </si>
+  <si>
+    <t>IN PARAM_CFNNC</t>
+  </si>
+  <si>
+    <t>IN PARAM_CSCRS</t>
+  </si>
+  <si>
+    <t>IN PARAM_CALMCM</t>
+  </si>
+  <si>
+    <t>IN PARAM_CMNDA</t>
+  </si>
+  <si>
+    <t>IN PARAM_CRGMN</t>
+  </si>
+  <si>
+    <t>IN PARAM_SIMPR</t>
+  </si>
+  <si>
+    <t>NUMERIC(8,0),</t>
+  </si>
+  <si>
+    <t>IN PARAM_CADNA</t>
+  </si>
+  <si>
+    <t>NUMERIC (6,0)  ,</t>
+  </si>
+  <si>
+    <t>IN PARAM_NANDCL</t>
+  </si>
+  <si>
+    <t>NUMERIC (4,0)  ,</t>
+  </si>
+  <si>
+    <t>IN PARAM_NPDDUA</t>
+  </si>
+  <si>
+    <t>NUMERIC (10,0)  ,</t>
+  </si>
+  <si>
+    <t>IN PARAM_SSTCOP</t>
+  </si>
+  <si>
+    <t>IN PARAM_SDBEND</t>
+  </si>
+  <si>
+    <t>IN PARAM_CCLNT1</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Código de compañía – Alfanumérico (2)</t>
+  </si>
+  <si>
+    <t>Código de división – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>Código de planta – Numérico (3,0)</t>
+  </si>
+  <si>
+    <t>Numero de Pre-Operación  - Numérico (10, 0)</t>
+  </si>
+  <si>
+    <t>Código tipo de operación – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>Código tipo almacén – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>Código del Cliente – Numérico (6, 0)</t>
+  </si>
+  <si>
+    <t>Código de Financiador – Numérico (4,0)</t>
+  </si>
+  <si>
+    <t>Código de sucursal -  Numérico (4,0)</t>
+  </si>
+  <si>
+    <t>Código de Almacén – Numérico (6,0)</t>
+  </si>
+  <si>
+    <t>Código de moneda – Numérico (3,0)</t>
+  </si>
+  <si>
+    <t>Código de régimen – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>Flag control Insumo-Producto – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>Flag impresión – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>Fecha Creación – Numérico(8,0)</t>
+  </si>
+  <si>
+    <t>Hora Creación – Numérico (6,0)</t>
+  </si>
+  <si>
+    <t>Usuario creador del registro – Alfanumérico (10)</t>
+  </si>
+  <si>
+    <t>Flag estado registro – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>·      CCMPN</t>
+  </si>
+  <si>
+    <t>·      CDVSN</t>
+  </si>
+  <si>
+    <t>·      CPLNDV</t>
+  </si>
+  <si>
+    <t>·      NPROPR</t>
+  </si>
+  <si>
+    <t>·      CTOPRC</t>
+  </si>
+  <si>
+    <t>·      CTPOAL</t>
+  </si>
+  <si>
+    <t>·      CCLNT</t>
+  </si>
+  <si>
+    <t>·      CFNNC</t>
+  </si>
+  <si>
+    <t>·      CSCRS</t>
+  </si>
+  <si>
+    <t>·      CALMCM</t>
+  </si>
+  <si>
+    <t>·      CMNDA</t>
+  </si>
+  <si>
+    <t>·      CRGMN</t>
+  </si>
+  <si>
+    <t>·      SCNINP</t>
+  </si>
+  <si>
+    <t>·      SIMPR</t>
+  </si>
+  <si>
+    <t>·      FCHCRT</t>
+  </si>
+  <si>
+    <t>·      HRACRT</t>
+  </si>
+  <si>
+    <t>·      USRCRT</t>
+  </si>
+  <si>
+    <t>·      SESTRG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de Aduana – Numérico (6,0)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Año declaración DUA – Numérico (4,0)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número pedido  depósito DUA – Numérico (10,0)  </t>
+  </si>
+  <si>
+    <t>Flag situación de operación – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>Flag doble endoso -  Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>Código Cliente</t>
+  </si>
+  <si>
+    <t>- Numérico (6,0)</t>
+  </si>
+  <si>
+    <t>·      CADNA</t>
+  </si>
+  <si>
+    <t>·      NANDCL</t>
+  </si>
+  <si>
+    <t>·      NPDDUA</t>
+  </si>
+  <si>
+    <t>·      SSTCOP</t>
+  </si>
+  <si>
+    <t>·      SDBEND</t>
+  </si>
+  <si>
+    <t>·      CCLNT1</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>Parametro procedure</t>
+  </si>
+  <si>
+    <t>Parametro documento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,13 +312,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -216,8 +347,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,18 +707,18 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f t="shared" ref="A2:A15" si="0">+CONCATENATE(B2," ",C2)</f>
-        <v>IN PARAM_NPROPR NUMERIC (10, 0),</v>
+        <f t="shared" ref="A2:A10" si="0">+CONCATENATE(B2," ",C2)</f>
+        <v>IN PARAM_NSLCPR NUMERIC (10, 0),</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F26" si="1">+MID(A2,4,LEN(A2)-2)</f>
-        <v>PARAM_NPROPR NUMERIC (10, 0),</v>
+        <v>PARAM_NSLCPR NUMERIC (10, 0),</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G26" si="2">+FIND(" ",F2,1)</f>
@@ -587,31 +726,31 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H26" si="3">+MID(F2,1,G2)</f>
-        <v xml:space="preserve">PARAM_NPROPR </v>
+        <v xml:space="preserve">PARAM_NSLCPR </v>
       </c>
       <c r="I2" t="str">
         <f t="shared" ref="I2:I26" si="4">IF(ISERR(FIND("NUMERIC",A2,1)),H2,CONCATENATE("CAST(",H2," AS VARCHAR(2000))"))</f>
-        <v>CAST(PARAM_NPROPR  AS VARCHAR(2000))</v>
+        <v>CAST(PARAM_NSLCPR  AS VARCHAR(2000))</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" ref="M2:M26" si="5">+CONCATENATE("'",H2,": '"," CONCAT ",I2, " CONCAT ' | ' CONCAT")</f>
-        <v>'PARAM_NPROPR : ' CONCAT CAST(PARAM_NPROPR  AS VARCHAR(2000)) CONCAT ' | ' CONCAT</v>
+        <v>'PARAM_NSLCPR : ' CONCAT CAST(PARAM_NSLCPR  AS VARCHAR(2000)) CONCAT ' | ' CONCAT</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_STPENT NUMERIC (5,0),</v>
+        <v>IN PARAM_SESTRG CHAR (1),</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="1"/>
-        <v>PARAM_STPENT NUMERIC (5,0),</v>
+        <v>PARAM_SESTRG CHAR (1),</v>
       </c>
       <c r="G3">
         <f t="shared" si="2"/>
@@ -619,278 +758,234 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_STPENT </v>
+        <v xml:space="preserve">PARAM_SESTRG </v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="4"/>
-        <v>CAST(PARAM_STPENT  AS VARCHAR(2000))</v>
+        <v xml:space="preserve">PARAM_SESTRG </v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="5"/>
-        <v>'PARAM_STPENT : ' CONCAT CAST(PARAM_STPENT  AS VARCHAR(2000)) CONCAT ' | ' CONCAT</v>
+        <v>'PARAM_SESTRG : ' CONCAT PARAM_SESTRG  CONCAT ' | ' CONCAT</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_CENTD NUMERIC (6,0),</v>
+        <v>IN PARAM_CULUSA CHAR (10),</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
-        <v>PARAM_CENTD NUMERIC (6,0),</v>
+        <v>PARAM_CULUSA CHAR (10),</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_CENTD </v>
+        <v xml:space="preserve">PARAM_CULUSA </v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="4"/>
-        <v>CAST(PARAM_CENTD  AS VARCHAR(2000))</v>
+        <v xml:space="preserve">PARAM_CULUSA </v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="5"/>
-        <v>'PARAM_CENTD : ' CONCAT CAST(PARAM_CENTD  AS VARCHAR(2000)) CONCAT ' | ' CONCAT</v>
+        <v>'PARAM_CULUSA : ' CONCAT PARAM_CULUSA  CONCAT ' | ' CONCAT</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_CRPRS CHAR (5),</v>
+        <v>IN PARAM_NTRMNL CHAR  (10),</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
-        <v>PARAM_CRPRS CHAR (5),</v>
+        <v>PARAM_NTRMNL CHAR  (10),</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_CRPRS </v>
+        <v xml:space="preserve">PARAM_NTRMNL </v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">PARAM_CRPRS </v>
+        <v xml:space="preserve">PARAM_NTRMNL </v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="5"/>
-        <v>'PARAM_CRPRS : ' CONCAT PARAM_CRPRS  CONCAT ' | ' CONCAT</v>
+        <v>'PARAM_NTRMNL : ' CONCAT PARAM_NTRMNL  CONCAT ' | ' CONCAT</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_NOPRCN NUMERIC (10, 0),</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="1"/>
-        <v>PARAM_NOPRCN NUMERIC (10, 0),</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_NOPRCN </v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="4"/>
-        <v>CAST(PARAM_NOPRCN  AS VARCHAR(2000))</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="5"/>
-        <v>'PARAM_NOPRCN : ' CONCAT CAST(PARAM_NOPRCN  AS VARCHAR(2000)) CONCAT ' | ' CONCAT</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F6" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G6" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H6" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M6" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_SFRMRP CHAR (1),</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="1"/>
-        <v>PARAM_SFRMRP CHAR (1),</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_SFRMRP </v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">PARAM_SFRMRP </v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="5"/>
-        <v>'PARAM_SFRMRP : ' CONCAT PARAM_SFRMRP  CONCAT ' | ' CONCAT</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F7" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G7" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I7" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M7" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_FFRMRP NUMERIC (8,0),</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="1"/>
-        <v>PARAM_FFRMRP NUMERIC (8,0),</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_FFRMRP </v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="4"/>
-        <v>CAST(PARAM_FFRMRP  AS VARCHAR(2000))</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="5"/>
-        <v>'PARAM_FFRMRP : ' CONCAT CAST(PARAM_FFRMRP  AS VARCHAR(2000)) CONCAT ' | ' CONCAT</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F8" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G8" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H8" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I8" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M8" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_HFRMRP NUMERIC (6,0),</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="1"/>
-        <v>PARAM_HFRMRP NUMERIC (6,0),</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_HFRMRP </v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="4"/>
-        <v>CAST(PARAM_HFRMRP  AS VARCHAR(2000))</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="5"/>
-        <v>'PARAM_HFRMRP : ' CONCAT CAST(PARAM_HFRMRP  AS VARCHAR(2000)) CONCAT ' | ' CONCAT</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F9" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G9" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H9" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I9" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M9" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_SESTRG CHAR (1) ,</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="1"/>
-        <v>PARAM_SESTRG CHAR (1) ,</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_SESTRG </v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">PARAM_SESTRG </v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" si="5"/>
-        <v>'PARAM_SESTRG : ' CONCAT PARAM_SESTRG  CONCAT ' | ' CONCAT</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F10" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G10" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H10" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M10" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_CULUSA CHAR (10),</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="1"/>
-        <v>PARAM_CULUSA CHAR (10),</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">PARAM_CULUSA </v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">PARAM_CULUSA </v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" si="5"/>
-        <v>'PARAM_CULUSA : ' CONCAT PARAM_CULUSA  CONCAT ' | ' CONCAT</v>
+      <c r="F11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I11" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M11" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="F12" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -913,10 +1008,6 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="F13" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -939,10 +1030,6 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="F14" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -965,10 +1052,6 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="F15" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -1013,6 +1096,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" ref="A2:A18" si="6">+CONCATENATE(B17," ",C17)</f>
+        <v xml:space="preserve"> </v>
+      </c>
       <c r="F17" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -1035,6 +1122,10 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
       <c r="F18" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -1167,10 +1258,6 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f t="shared" ref="A2:A25" si="6">+CONCATENATE(B24," ",C24)</f>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="F24" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -1194,7 +1281,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="A5:A27" si="7">+CONCATENATE(B25," ",C25)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F25" t="e">
@@ -1219,6 +1306,10 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> </v>
+      </c>
       <c r="F26" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
@@ -1238,6 +1329,12 @@
       <c r="M26" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1253,184 +1350,757 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="A1:B22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="4"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="str">
+        <f>+CONCATENATE(B2," ",C2)</f>
+        <v>IN PARAM_CCMPN CHAR (2),</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" t="str">
+        <f>+MID(F2,8,LEN(F2)-7)</f>
+        <v>CCMPN</v>
+      </c>
+      <c r="N2" s="1">
+        <f>IF(ISERROR(FIND(M2,A2,1)),0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
+        <f t="shared" ref="A3:A25" si="0">+CONCATENATE(B3," ",C3)</f>
+        <v>IN PARAM_CDVSN CHAR (1),</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M25" si="1">+MID(F3,8,LEN(F3)-7)</f>
+        <v>CDVSN</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" ref="N3:N25" si="2">IF(ISERROR(FIND(M3,A3,1)),0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CPLNDV NUMERIC (3,0),</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>CPLNDV</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_NPROPR NUMERIC (10, 0),</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>NPROPR</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CTOPRC CHAR (1),</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>CTOPRC</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CTPOAL CHAR (1),</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>CTPOAL</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CCLNT NUMERIC (6, 0),</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>CCLNT</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CFNNC NUMERIC (4,0),</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>CFNNC</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CSCRS NUMERIC (4,0),</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>CSCRS</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CALMCM NUMERIC (6,0),</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>CALMCM</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CMNDA NUMERIC (3,0),</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>CMNDA</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CRGMN CHAR (1) ,</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>CRGMN</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_SCNINP CHAR (1),</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>SCNINP</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_SIMPR CHAR (1),</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>SIMPR</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_FCHCRT NUMERIC(8,0),</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>FCHCRT</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_HRACRT NUMERIC (6,0),</v>
+      </c>
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>HRACRT</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_USRCRT CHAR (10),</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>USRCRT</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_SESTRG CHAR (1),</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>SESTRG</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CADNA NUMERIC (6,0)  ,</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>78</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>CADNA</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_NANDCL NUMERIC (4,0)  ,</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
+        <v>79</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>NANDCL</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_NPDDUA NUMERIC (10,0)  ,</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="F22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
+        <v>80</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>NPDDUA</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_SSTCOP CHAR (1),</v>
+      </c>
+      <c r="B23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" t="s">
+        <v>81</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="1"/>
+        <v>SSTCOP</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_SDBEND CHAR (1),</v>
+      </c>
+      <c r="B24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" t="s">
+        <v>82</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="1"/>
+        <v>SDBEND</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PARAM_CCLNT1 NUMERIC (6,0),</v>
+      </c>
+      <c r="B25" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" t="s">
+        <v>84</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="1"/>
+        <v>CCLNT1</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="120" verticalDpi="72" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{44349F47-1EA6-4AE5-B37D-50F8A29B1056}">
+            <x14:iconSet showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="3"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>N2:N25</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cambios realizado por cambios en espesificacion de documento
</commit_message>
<xml_diff>
--- a/Otros (Plantillas, etc)/plantilla codigo.xlsx
+++ b/Otros (Plantillas, etc)/plantilla codigo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Generador Parametros" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>IN PARAM_CCMPN</t>
   </si>
@@ -30,9 +30,6 @@
     <t>CHAR (1),</t>
   </si>
   <si>
-    <t>IN PARAM_CPLNDV</t>
-  </si>
-  <si>
     <t>IN PARAM_NPROPR</t>
   </si>
   <si>
@@ -42,21 +39,9 @@
     <t>CHAR (10),</t>
   </si>
   <si>
-    <t>IN PARAM_SCNINP</t>
-  </si>
-  <si>
     <t>IN PARAM_SESTRG</t>
   </si>
   <si>
-    <t>NUMERIC (6,0),</t>
-  </si>
-  <si>
-    <t>IN PARAM_FCHCRT</t>
-  </si>
-  <si>
-    <t>IN PARAM_HRACRT</t>
-  </si>
-  <si>
     <t>IN PARAM_CULUSA</t>
   </si>
   <si>
@@ -69,12 +54,6 @@
     <t>IN PARAM_NTRMNL</t>
   </si>
   <si>
-    <t>NUMERIC (3,0),</t>
-  </si>
-  <si>
-    <t>NUMERIC(8,0),</t>
-  </si>
-  <si>
     <t>:</t>
   </si>
   <si>
@@ -84,51 +63,21 @@
     <t>Código de división – Alfanumérico (1)</t>
   </si>
   <si>
-    <t>Código de planta – Numérico (3,0)</t>
-  </si>
-  <si>
     <t>Código de régimen – Alfanumérico (1)</t>
   </si>
   <si>
-    <t>Flag control Insumo-Producto – Alfanumérico (1)</t>
-  </si>
-  <si>
-    <t>Fecha Creación – Numérico(8,0)</t>
-  </si>
-  <si>
-    <t>Hora Creación – Numérico (6,0)</t>
-  </si>
-  <si>
-    <t>Flag estado registro – Alfanumérico (1)</t>
-  </si>
-  <si>
     <t>·      CCMPN</t>
   </si>
   <si>
     <t>·      CDVSN</t>
   </si>
   <si>
-    <t>·      CPLNDV</t>
-  </si>
-  <si>
     <t>·      NPROPR</t>
   </si>
   <si>
     <t>·      CRGMN</t>
   </si>
   <si>
-    <t>·      SCNINP</t>
-  </si>
-  <si>
-    <t>·      FCHCRT</t>
-  </si>
-  <si>
-    <t>·      HRACRT</t>
-  </si>
-  <si>
-    <t>·      SESTRG</t>
-  </si>
-  <si>
     <t>Match</t>
   </si>
   <si>
@@ -138,9 +87,6 @@
     <t>Parametro documento</t>
   </si>
   <si>
-    <t>IN PARAM_CRGMN CHAR(1),</t>
-  </si>
-  <si>
     <t>IN PARAM_NITEM</t>
   </si>
   <si>
@@ -156,54 +102,24 @@
     <t>IN PARAM_STPCNS</t>
   </si>
   <si>
-    <t xml:space="preserve">CHAR (1), </t>
-  </si>
-  <si>
     <t>IN PARAM_CFMLPR</t>
   </si>
   <si>
     <t>CHAR (2) ,</t>
   </si>
   <si>
-    <t>IN PARAM_CUSCRT</t>
-  </si>
-  <si>
-    <t>IN PARAM_NTRMCR</t>
-  </si>
-  <si>
     <t>IN PARAM_NSRIE1</t>
   </si>
   <si>
-    <t>NUMERIC (6,0) ,</t>
-  </si>
-  <si>
     <t>IN PARAM_NDCMSS</t>
   </si>
   <si>
     <t>NUMERIC (10,0) ,</t>
   </si>
   <si>
-    <t>IN PARAM_IVUNIT NUMERIC ( 15, 5 ),</t>
-  </si>
-  <si>
-    <t>IN PARAM_IVTOIT NUMERIC ( 15,5 ),</t>
-  </si>
-  <si>
-    <t>IN PARAM_CANTIDAD NUMERIC (15,5) ,</t>
-  </si>
-  <si>
     <t>IN PARAM_UNIDAD</t>
   </si>
   <si>
-    <t xml:space="preserve">CHAR (3), </t>
-  </si>
-  <si>
-    <t>Número de Pre-Operación  - Numérico (10, 0)</t>
-  </si>
-  <si>
-    <t>Número de Item – Numérico (5,0)</t>
-  </si>
-  <si>
     <t>Código del Producto – Alfanumérico (10)</t>
   </si>
   <si>
@@ -216,12 +132,6 @@
     <t>Código Familia del Producto – Alfanumérico (2)</t>
   </si>
   <si>
-    <t>Código usuario creador – Alfanumérico (10)</t>
-  </si>
-  <si>
-    <t>Numero Terminal Usado – Alfanumérico  (10)</t>
-  </si>
-  <si>
     <t>·      NITEM</t>
   </si>
   <si>
@@ -237,12 +147,6 @@
     <t>·      CFMLPR</t>
   </si>
   <si>
-    <t>·      CUSCRT</t>
-  </si>
-  <si>
-    <t>·      NTRMCR</t>
-  </si>
-  <si>
     <t>Número de serie – Numérico (6,0) .</t>
   </si>
   <si>
@@ -264,12 +168,6 @@
     <t>·      NDCMSS</t>
   </si>
   <si>
-    <t xml:space="preserve">·      IVUNIT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">·      IVTOIT </t>
-  </si>
-  <si>
     <t xml:space="preserve">Cantidad solicitada – Numérico (15,5) </t>
   </si>
   <si>
@@ -277,6 +175,60 @@
   </si>
   <si>
     <t>·      CANTIDAD</t>
+  </si>
+  <si>
+    <t>IN PARAM_CRGMN</t>
+  </si>
+  <si>
+    <t>CHAR (1) ,</t>
+  </si>
+  <si>
+    <t>NUMERIC (6,0)  ,</t>
+  </si>
+  <si>
+    <t>IN PARAM_IVUNIT</t>
+  </si>
+  <si>
+    <t>NUMERIC ( 15, 5 ),</t>
+  </si>
+  <si>
+    <t>IN PARAM_IVTOIT</t>
+  </si>
+  <si>
+    <t>NUMERIC ( 15,5 ),</t>
+  </si>
+  <si>
+    <t>IN PARAM_CANTIDAD</t>
+  </si>
+  <si>
+    <t>NUMERIC (15,5) ,</t>
+  </si>
+  <si>
+    <t>CHAR (3) ,</t>
+  </si>
+  <si>
+    <t>IN PARAM_SCNINP CHAR(1),--EN ESPERA DE CONFIRMACION</t>
+  </si>
+  <si>
+    <t>IN PARAM_SCNINP CHAR(1),</t>
+  </si>
+  <si>
+    <t>Numero de Pre-Operación  - Numérico (10, 0)</t>
+  </si>
+  <si>
+    <t>·      CULUSA</t>
+  </si>
+  <si>
+    <t>Código usuario actualizador – Alfanumérico (10)</t>
+  </si>
+  <si>
+    <t>Numero de Item – Numérico (5,0)</t>
+  </si>
+  <si>
+    <t>·      IVUNIT</t>
+  </si>
+  <si>
+    <t>·      IVTOIT</t>
   </si>
 </sst>
 </file>
@@ -690,10 +642,10 @@
         <v>IN PARAM_NSLCPR NUMERIC (10, 0),</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F26" si="1">+MID(A2,4,LEN(A2)-2)</f>
@@ -722,7 +674,7 @@
         <v>IN PARAM_SESTRG CHAR (1),</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -754,10 +706,10 @@
         <v>IN PARAM_CULUSA CHAR (10),</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -786,10 +738,10 @@
         <v>IN PARAM_NTRMNL CHAR  (10),</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1329,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,13 +1297,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1366,13 +1318,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="M2" t="str">
         <f>+MID(F2,8,LEN(F2)-7)</f>
@@ -1385,7 +1337,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
-        <f t="shared" ref="A3:A24" si="0">+CONCATENATE(B3," ",C3)</f>
+        <f t="shared" ref="A3:A17" si="0">+CONCATENATE(B3," ",C3)</f>
         <v>IN PARAM_CDVSN CHAR (1),</v>
       </c>
       <c r="B3" t="s">
@@ -1395,46 +1347,46 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M24" si="1">+MID(F3,8,LEN(F3)-7)</f>
+        <f t="shared" ref="M3:M23" si="1">+MID(F3,8,LEN(F3)-7)</f>
         <v>CDVSN</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N24" si="2">IF(ISERROR(FIND(M3,A3,1)),0,1)</f>
+        <f t="shared" ref="N3:N23" si="2">IF(ISERROR(FIND(M3,A3,1)),0,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_CPLNDV NUMERIC (3,0),</v>
+        <v>IN PARAM_NPROPR NUMERIC (10, 0),</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v>CPLNDV</v>
+        <v>NPROPR</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" si="2"/>
@@ -1444,23 +1396,26 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">IN PARAM_CRGMN CHAR(1), </v>
+        <v>IN PARAM_NITEM NUMERIC (5,0),</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="1"/>
-        <v>CRGMN</v>
+        <v>NITEM</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="2"/>
@@ -1470,26 +1425,26 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_NPROPR NUMERIC (10, 0),</v>
+        <v>IN PARAM_CDPRDC CHAR (10),</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="1"/>
-        <v>NPROPR</v>
+        <v>CDPRDC</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="2"/>
@@ -1499,26 +1454,26 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_NITEM NUMERIC (5,0),</v>
+        <v>IN PARAM_CRGMN CHAR (1) ,</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v>NITEM</v>
+        <v>CRGMN</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="2"/>
@@ -1528,26 +1483,26 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_CDPRDC CHAR (10),</v>
+        <v>IN PARAM_SINSPR CHAR (1),</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="1"/>
-        <v>CDPRDC</v>
+        <v>SINSPR</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="2"/>
@@ -1557,26 +1512,26 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_SINSPR CHAR (1),</v>
+        <v>IN PARAM_STPCNS CHAR (1) ,</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v>SINSPR</v>
+        <v>STPCNS</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="2"/>
@@ -1586,26 +1541,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_SCNINP CHAR (1),</v>
+        <v>IN PARAM_CFMLPR CHAR (2) ,</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v>SCNINP</v>
+        <v>CFMLPR</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="2"/>
@@ -1615,26 +1570,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">IN PARAM_STPCNS CHAR (1), </v>
+        <v>IN PARAM_CULUSA CHAR (10),</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
-        <v>STPCNS</v>
+        <v>CULUSA</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="2"/>
@@ -1644,26 +1599,26 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_CFMLPR CHAR (2) ,</v>
+        <v>IN PARAM_NSRIE1 NUMERIC (6,0)  ,</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
-        <v>CFMLPR</v>
+        <v>NSRIE1</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="2"/>
@@ -1673,26 +1628,26 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_FCHCRT NUMERIC(8,0),</v>
+        <v>IN PARAM_NDCMSS NUMERIC (10,0) ,</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
-        <v>FCHCRT</v>
+        <v>NDCMSS</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="2"/>
@@ -1702,26 +1657,26 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_HRACRT NUMERIC (6,0),</v>
+        <v>IN PARAM_IVUNIT NUMERIC ( 15, 5 ),</v>
       </c>
       <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" t="s">
-        <v>19</v>
-      </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
-        <v>HRACRT</v>
+        <v>IVUNIT</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="2"/>
@@ -1731,26 +1686,26 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_CUSCRT CHAR (10),</v>
+        <v>IN PARAM_IVTOIT NUMERIC ( 15,5 ),</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
-        <v>CUSCRT</v>
+        <v>IVTOIT</v>
       </c>
       <c r="N15" s="1">
         <f t="shared" si="2"/>
@@ -1760,26 +1715,26 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_NTRMCR CHAR  (10),</v>
+        <v>IN PARAM_CANTIDAD NUMERIC (15,5) ,</v>
       </c>
       <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
         <v>50</v>
       </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" t="s">
-        <v>67</v>
-      </c>
       <c r="M16" t="str">
         <f t="shared" si="1"/>
-        <v>NTRMCR</v>
+        <v>CANTIDAD</v>
       </c>
       <c r="N16" s="1">
         <f t="shared" si="2"/>
@@ -1789,26 +1744,26 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>IN PARAM_SESTRG CHAR (1),</v>
+        <v>IN PARAM_UNIDAD CHAR (3) ,</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
-        <v>SESTRG</v>
+        <v>UNIDAD</v>
       </c>
       <c r="N17" s="1">
         <f t="shared" si="2"/>
@@ -1816,180 +1771,67 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_NSRIE1 NUMERIC (6,0) ,</v>
+      <c r="A18" t="s">
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" t="s">
-        <v>75</v>
-      </c>
-      <c r="M18" t="str">
-        <f t="shared" si="1"/>
-        <v>NSRIE1</v>
+        <v>63</v>
+      </c>
+      <c r="M18" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N18" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_NDCMSS NUMERIC (10,0) ,</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" t="s">
-        <v>76</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" si="1"/>
-        <v>NDCMSS</v>
+      <c r="M19" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N19" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">IN PARAM_IVUNIT NUMERIC ( 15, 5 ), </v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" t="s">
-        <v>77</v>
-      </c>
-      <c r="M20" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">IVUNIT </v>
+      <c r="M20" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N20" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">IN PARAM_IVTOIT NUMERIC ( 15,5 ), </v>
-      </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" t="s">
-        <v>78</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">IVTOIT </v>
+      <c r="M21" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N21" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">IN PARAM_CANTIDAD NUMERIC (15,5) , </v>
-      </c>
-      <c r="B22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" t="s">
-        <v>84</v>
-      </c>
-      <c r="M22" t="str">
-        <f t="shared" si="1"/>
-        <v>CANTIDAD</v>
+      <c r="M22" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">IN PARAM_UNIDAD CHAR (3), </v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" t="s">
-        <v>79</v>
-      </c>
-      <c r="M23" t="str">
-        <f t="shared" si="1"/>
-        <v>UNIDAD</v>
+      <c r="M23" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="M24" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N24" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2001,7 +1843,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{44349F47-1EA6-4AE5-B37D-50F8A29B1056}">
+          <x14:cfRule type="iconSet" priority="3" id="{44349F47-1EA6-4AE5-B37D-50F8A29B1056}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -2017,7 +1859,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>N2:N24</xm:sqref>
+          <xm:sqref>N2:N23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Cambios realizados a Warrants segun correo 20171213 1628
</commit_message>
<xml_diff>
--- a/Otros (Plantillas, etc)/plantilla codigo.xlsx
+++ b/Otros (Plantillas, etc)/plantilla codigo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>IN PARAM_CCMPN</t>
   </si>
@@ -24,9 +24,6 @@
     <t>CHAR (2),</t>
   </si>
   <si>
-    <t>IN PARAM_CDVSN</t>
-  </si>
-  <si>
     <t>CHAR (1),</t>
   </si>
   <si>
@@ -60,18 +57,12 @@
     <t>Código de compañía – Alfanumérico (2)</t>
   </si>
   <si>
-    <t>Código de división – Alfanumérico (1)</t>
-  </si>
-  <si>
     <t>Código de régimen – Alfanumérico (1)</t>
   </si>
   <si>
     <t>·      CCMPN</t>
   </si>
   <si>
-    <t>·      CDVSN</t>
-  </si>
-  <si>
     <t>·      NPROPR</t>
   </si>
   <si>
@@ -93,126 +84,24 @@
     <t>NUMERIC (5,0),</t>
   </si>
   <si>
-    <t>IN PARAM_CDPRDC</t>
-  </si>
-  <si>
-    <t>IN PARAM_SINSPR</t>
-  </si>
-  <si>
     <t>IN PARAM_STPCNS</t>
   </si>
   <si>
-    <t>IN PARAM_CFMLPR</t>
-  </si>
-  <si>
-    <t>CHAR (2) ,</t>
-  </si>
-  <si>
-    <t>IN PARAM_NSRIE1</t>
-  </si>
-  <si>
-    <t>IN PARAM_NDCMSS</t>
-  </si>
-  <si>
-    <t>NUMERIC (10,0) ,</t>
-  </si>
-  <si>
-    <t>IN PARAM_UNIDAD</t>
-  </si>
-  <si>
-    <t>Código del Producto – Alfanumérico (10)</t>
-  </si>
-  <si>
-    <t>Flag Insumo / Producto – Alfanumérico (1)</t>
-  </si>
-  <si>
     <t>Flag tipo de Control Serie -  Alfanumérico (1)</t>
   </si>
   <si>
-    <t>Código Familia del Producto – Alfanumérico (2)</t>
-  </si>
-  <si>
     <t>·      NITEM</t>
   </si>
   <si>
-    <t>·      CDPRDC</t>
-  </si>
-  <si>
-    <t>·      SINSPR</t>
-  </si>
-  <si>
     <t>·      STPCNS</t>
   </si>
   <si>
-    <t>·      CFMLPR</t>
-  </si>
-  <si>
-    <t>Número de serie – Numérico (6,0) .</t>
-  </si>
-  <si>
-    <t>Número documento Sustento – Numérico (10,0).</t>
-  </si>
-  <si>
-    <t>Importe unitario del ítem – Numérico ( 15, 5 ).</t>
-  </si>
-  <si>
-    <t>Importe valor total del ítem – Numérico ( 15,5 ).</t>
-  </si>
-  <si>
-    <t>Unidad solicitada -  Alfanumérico (3)</t>
-  </si>
-  <si>
-    <t>·      NSRIE1</t>
-  </si>
-  <si>
-    <t>·      NDCMSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cantidad solicitada – Numérico (15,5) </t>
-  </si>
-  <si>
-    <t>·      UNIDAD</t>
-  </si>
-  <si>
-    <t>·      CANTIDAD</t>
-  </si>
-  <si>
     <t>IN PARAM_CRGMN</t>
   </si>
   <si>
     <t>CHAR (1) ,</t>
   </si>
   <si>
-    <t>NUMERIC (6,0)  ,</t>
-  </si>
-  <si>
-    <t>IN PARAM_IVUNIT</t>
-  </si>
-  <si>
-    <t>NUMERIC ( 15, 5 ),</t>
-  </si>
-  <si>
-    <t>IN PARAM_IVTOIT</t>
-  </si>
-  <si>
-    <t>NUMERIC ( 15,5 ),</t>
-  </si>
-  <si>
-    <t>IN PARAM_CANTIDAD</t>
-  </si>
-  <si>
-    <t>NUMERIC (15,5) ,</t>
-  </si>
-  <si>
-    <t>CHAR (3) ,</t>
-  </si>
-  <si>
-    <t>IN PARAM_SCNINP CHAR(1),--EN ESPERA DE CONFIRMACION</t>
-  </si>
-  <si>
-    <t>IN PARAM_SCNINP CHAR(1),</t>
-  </si>
-  <si>
     <t>Numero de Pre-Operación  - Numérico (10, 0)</t>
   </si>
   <si>
@@ -225,10 +114,70 @@
     <t>Numero de Item – Numérico (5,0)</t>
   </si>
   <si>
-    <t>·      IVUNIT</t>
-  </si>
-  <si>
-    <t>·      IVTOIT</t>
+    <t>·      SESTRG</t>
+  </si>
+  <si>
+    <t>Flag estado registro – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>NUMERIC (15,5),</t>
+  </si>
+  <si>
+    <t>IN PARAM_QSLPSF</t>
+  </si>
+  <si>
+    <t>·      QSLPSF</t>
+  </si>
+  <si>
+    <t>IN PARAM_QSLCNF</t>
+  </si>
+  <si>
+    <t>IN PARAM_QSLCND</t>
+  </si>
+  <si>
+    <t>NUMERIC (15, 5),</t>
+  </si>
+  <si>
+    <t>IN PARAM_QSLPSD</t>
+  </si>
+  <si>
+    <t>IN PARAM_ISLDFN</t>
+  </si>
+  <si>
+    <t>IN PARAM_ISLDDC</t>
+  </si>
+  <si>
+    <t>·      QSLCNF</t>
+  </si>
+  <si>
+    <t>Saldo cantidad financiera – Decimal (15,5)</t>
+  </si>
+  <si>
+    <t>·      QSLCND</t>
+  </si>
+  <si>
+    <t>Saldo cantidad declarada – Decimal (15,5)</t>
+  </si>
+  <si>
+    <t>Saldo peso financiero – Decimal (15, 5)</t>
+  </si>
+  <si>
+    <t>·      QSLPSD</t>
+  </si>
+  <si>
+    <t>Saldo peso declarado – Decimal (15,5)</t>
+  </si>
+  <si>
+    <t>·      ISLDFN</t>
+  </si>
+  <si>
+    <t>Importe saldo financiero – Decimal (15,5)</t>
+  </si>
+  <si>
+    <t>·      ISLDDC</t>
+  </si>
+  <si>
+    <t>Importe saldo declarado – Numérico (15,5)</t>
   </si>
 </sst>
 </file>
@@ -642,10 +591,10 @@
         <v>IN PARAM_NSLCPR NUMERIC (10, 0),</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F26" si="1">+MID(A2,4,LEN(A2)-2)</f>
@@ -674,10 +623,10 @@
         <v>IN PARAM_SESTRG CHAR (1),</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="1"/>
@@ -706,10 +655,10 @@
         <v>IN PARAM_CULUSA CHAR (10),</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -738,10 +687,10 @@
         <v>IN PARAM_NTRMNL CHAR  (10),</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1281,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,19 +1246,18 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="str">
-        <f>+CONCATENATE(B2," ",C2)</f>
-        <v>IN PARAM_CCMPN CHAR (2),</v>
+      <c r="A2" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1318,13 +1266,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
       </c>
       <c r="M2" t="str">
         <f>+MID(F2,8,LEN(F2)-7)</f>
@@ -1336,503 +1284,488 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="str">
-        <f t="shared" ref="A3:A17" si="0">+CONCATENATE(B3," ",C3)</f>
-        <v>IN PARAM_CDVSN CHAR (1),</v>
+      <c r="A3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M23" si="0">+MID(F3,8,LEN(F3)-7)</f>
+        <v>NPROPR</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" ref="N3:N29" si="1">IF(ISERROR(FIND(M3,A3,1)),0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>NITEM</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>CRGMN</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>STPCNS</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>QSLCNF</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>QSLCND</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>QSLPSF</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>QSLPSD</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>ISLDFN</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>ISLDDC</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M23" si="1">+MID(F3,8,LEN(F3)-7)</f>
-        <v>CDVSN</v>
-      </c>
-      <c r="N3" s="1">
-        <f t="shared" ref="N3:N23" si="2">IF(ISERROR(FIND(M3,A3,1)),0,1)</f>
+      <c r="F13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>SESTRG</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_NPROPR NUMERIC (10, 0),</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" si="1"/>
-        <v>NPROPR</v>
-      </c>
-      <c r="N4" s="1">
-        <f t="shared" si="2"/>
+      <c r="F14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>CULUSA</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_NITEM NUMERIC (5,0),</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" si="1"/>
-        <v>NITEM</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_CDPRDC CHAR (10),</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="1"/>
-        <v>CDPRDC</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_CRGMN CHAR (1) ,</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="1"/>
-        <v>CRGMN</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_SINSPR CHAR (1),</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="1"/>
-        <v>SINSPR</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_STPCNS CHAR (1) ,</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="1"/>
-        <v>STPCNS</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_CFMLPR CHAR (2) ,</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" si="1"/>
-        <v>CFMLPR</v>
-      </c>
-      <c r="N10" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_CULUSA CHAR (10),</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" si="1"/>
-        <v>CULUSA</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_NSRIE1 NUMERIC (6,0)  ,</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" si="1"/>
-        <v>NSRIE1</v>
-      </c>
-      <c r="N12" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_NDCMSS NUMERIC (10,0) ,</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>44</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" si="1"/>
-        <v>NDCMSS</v>
-      </c>
-      <c r="N13" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_IVUNIT NUMERIC ( 15, 5 ),</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>45</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="1"/>
-        <v>IVUNIT</v>
-      </c>
-      <c r="N14" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_IVTOIT NUMERIC ( 15,5 ),</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" t="s">
-        <v>46</v>
-      </c>
-      <c r="M15" t="str">
-        <f t="shared" si="1"/>
-        <v>IVTOIT</v>
+      <c r="M15" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_CANTIDAD NUMERIC (15,5) ,</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" si="1"/>
-        <v>CANTIDAD</v>
+      <c r="M16" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PARAM_UNIDAD CHAR (3) ,</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="1"/>
-        <v>UNIDAD</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M17" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M18" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M19" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M20" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M21" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M22" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M23" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M24" t="e">
+        <f t="shared" ref="M24" si="2">+MID(F24,8,LEN(F24)-7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M25" t="e">
+        <f t="shared" ref="M25:M29" si="3">+MID(F25,8,LEN(F25)-7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M26" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M27" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M28" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M29" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1843,7 +1776,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{44349F47-1EA6-4AE5-B37D-50F8A29B1056}">
+          <x14:cfRule type="iconSet" priority="4" id="{44349F47-1EA6-4AE5-B37D-50F8A29B1056}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1859,7 +1792,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>N2:N23</xm:sqref>
+          <xm:sqref>N2:N29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Merge de scripts de prorrogas desarrollado por Humberto Arana
</commit_message>
<xml_diff>
--- a/Otros (Plantillas, etc)/plantilla codigo.xlsx
+++ b/Otros (Plantillas, etc)/plantilla codigo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>IN PARAM_CCMPN</t>
   </si>
@@ -57,18 +57,6 @@
     <t>Código de compañía – Alfanumérico (2)</t>
   </si>
   <si>
-    <t>Código de régimen – Alfanumérico (1)</t>
-  </si>
-  <si>
-    <t>·      CCMPN</t>
-  </si>
-  <si>
-    <t>·      NPROPR</t>
-  </si>
-  <si>
-    <t>·      CRGMN</t>
-  </si>
-  <si>
     <t>Match</t>
   </si>
   <si>
@@ -78,24 +66,6 @@
     <t>Parametro documento</t>
   </si>
   <si>
-    <t>IN PARAM_NITEM</t>
-  </si>
-  <si>
-    <t>NUMERIC (5,0),</t>
-  </si>
-  <si>
-    <t>IN PARAM_STPCNS</t>
-  </si>
-  <si>
-    <t>Flag tipo de Control Serie -  Alfanumérico (1)</t>
-  </si>
-  <si>
-    <t>·      NITEM</t>
-  </si>
-  <si>
-    <t>·      STPCNS</t>
-  </si>
-  <si>
     <t>IN PARAM_CRGMN</t>
   </si>
   <si>
@@ -105,79 +75,133 @@
     <t>Numero de Pre-Operación  - Numérico (10, 0)</t>
   </si>
   <si>
-    <t>·      CULUSA</t>
-  </si>
-  <si>
     <t>Código usuario actualizador – Alfanumérico (10)</t>
   </si>
   <si>
-    <t>Numero de Item – Numérico (5,0)</t>
-  </si>
-  <si>
-    <t>·      SESTRG</t>
-  </si>
-  <si>
-    <t>Flag estado registro – Alfanumérico (1)</t>
-  </si>
-  <si>
-    <t>NUMERIC (15,5),</t>
-  </si>
-  <si>
-    <t>IN PARAM_QSLPSF</t>
-  </si>
-  <si>
-    <t>·      QSLPSF</t>
-  </si>
-  <si>
-    <t>IN PARAM_QSLCNF</t>
-  </si>
-  <si>
-    <t>IN PARAM_QSLCND</t>
-  </si>
-  <si>
-    <t>NUMERIC (15, 5),</t>
-  </si>
-  <si>
-    <t>IN PARAM_QSLPSD</t>
-  </si>
-  <si>
-    <t>IN PARAM_ISLDFN</t>
-  </si>
-  <si>
-    <t>IN PARAM_ISLDDC</t>
-  </si>
-  <si>
-    <t>·      QSLCNF</t>
-  </si>
-  <si>
-    <t>Saldo cantidad financiera – Decimal (15,5)</t>
-  </si>
-  <si>
-    <t>·      QSLCND</t>
-  </si>
-  <si>
-    <t>Saldo cantidad declarada – Decimal (15,5)</t>
-  </si>
-  <si>
-    <t>Saldo peso financiero – Decimal (15, 5)</t>
-  </si>
-  <si>
-    <t>·      QSLPSD</t>
-  </si>
-  <si>
-    <t>Saldo peso declarado – Decimal (15,5)</t>
-  </si>
-  <si>
-    <t>·      ISLDFN</t>
-  </si>
-  <si>
-    <t>Importe saldo financiero – Decimal (15,5)</t>
-  </si>
-  <si>
-    <t>·      ISLDDC</t>
-  </si>
-  <si>
-    <t>Importe saldo declarado – Numérico (15,5)</t>
+    <t>IN PARAM_CTPOAL</t>
+  </si>
+  <si>
+    <t>IN PARAM_CFNNC</t>
+  </si>
+  <si>
+    <t>IN PARAM_CSCRS</t>
+  </si>
+  <si>
+    <t>IN PARAM_CALMCM</t>
+  </si>
+  <si>
+    <t>IN PARAM_CMNDA</t>
+  </si>
+  <si>
+    <t>IN PARAM_SIMPR</t>
+  </si>
+  <si>
+    <t>IN PARAM_CADNA</t>
+  </si>
+  <si>
+    <t>IN PARAM_NANDCL</t>
+  </si>
+  <si>
+    <t>IN PARAM_NPDDUA</t>
+  </si>
+  <si>
+    <t>CCMPN</t>
+  </si>
+  <si>
+    <t>NPROPR</t>
+  </si>
+  <si>
+    <t>CTPOAL</t>
+  </si>
+  <si>
+    <t>Código tipo almacén – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>CFNNC</t>
+  </si>
+  <si>
+    <t>Código de Financiador – Numérico (4,0)</t>
+  </si>
+  <si>
+    <t>CSCRS</t>
+  </si>
+  <si>
+    <t>Código de sucursal -  Numérico (4,0)</t>
+  </si>
+  <si>
+    <t>CALMCM</t>
+  </si>
+  <si>
+    <t>Código de Almacén – Numérico (6,0)</t>
+  </si>
+  <si>
+    <t>CMNDA</t>
+  </si>
+  <si>
+    <t>Código de moneda – Numérico (3,0)</t>
+  </si>
+  <si>
+    <t>CRGMN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de régimen – Alfanumérico (1) </t>
+  </si>
+  <si>
+    <t>SIMPR</t>
+  </si>
+  <si>
+    <t>Flag impresión – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>CADNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de Aduana – Numérico (6,0)  </t>
+  </si>
+  <si>
+    <t>NANDCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Año declaración DUA – Numérico (4,0)  </t>
+  </si>
+  <si>
+    <t>NPDDUA</t>
+  </si>
+  <si>
+    <t>CHAR (2) ,</t>
+  </si>
+  <si>
+    <t>NUMERIC (6,0) ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número pedido. depósito DUA– Numérico (10,0) </t>
+  </si>
+  <si>
+    <t>NUMERIC (6,0)   ,</t>
+  </si>
+  <si>
+    <t>NUMERIC (4,0)   ,</t>
+  </si>
+  <si>
+    <t>NUMERIC (10,0)   ,</t>
+  </si>
+  <si>
+    <t>CULUSA</t>
+  </si>
+  <si>
+    <t>NUMERIC (10, 0) ,</t>
+  </si>
+  <si>
+    <t>NUMERIC (3,0) ,</t>
+  </si>
+  <si>
+    <t>NUMERIC (4,0) ,</t>
+  </si>
+  <si>
+    <t>CHAR (1)  ,</t>
+  </si>
+  <si>
+    <t>CHAR (10) ,</t>
   </si>
 </sst>
 </file>
@@ -1230,29 +1254,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1263,23 +1287,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="str">
-        <f>+MID(F2,8,LEN(F2)-7)</f>
-        <v>CCMPN</v>
-      </c>
       <c r="N2" s="1">
-        <f>IF(ISERROR(FIND(M2,A2,1)),0,1)</f>
+        <f>IF(ISERROR(FIND(F2,A2,1)),0,IF(ISBLANK(F2),0,1))</f>
         <v>1</v>
       </c>
     </row>
@@ -1291,23 +1314,22 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M23" si="0">+MID(F3,8,LEN(F3)-7)</f>
-        <v>NPROPR</v>
+      <c r="I3" t="s">
+        <v>18</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N29" si="1">IF(ISERROR(FIND(M3,A3,1)),0,1)</f>
+        <f t="shared" ref="N3:N30" si="0">IF(ISERROR(FIND(F3,A3,1)),0,IF(ISBLANK(F3),0,1))</f>
         <v>1</v>
       </c>
     </row>
@@ -1319,454 +1341,413 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" si="0"/>
-        <v>NITEM</v>
+      <c r="I4" t="s">
+        <v>32</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" si="0"/>
-        <v>CRGMN</v>
+      <c r="I5" t="s">
+        <v>38</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="0"/>
-        <v>STPCNS</v>
+      <c r="I6" t="s">
+        <v>40</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="0"/>
-        <v>QSLCNF</v>
-      </c>
       <c r="N7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="0"/>
-        <v>QSLCND</v>
+      <c r="I8" t="s">
+        <v>36</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
         <v>11</v>
       </c>
-      <c r="H9" t="s">
-        <v>47</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="0"/>
-        <v>QSLPSF</v>
+      <c r="I9" t="s">
+        <v>42</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
         <v>11</v>
       </c>
-      <c r="H10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" si="0"/>
-        <v>QSLPSD</v>
+      <c r="I10" t="s">
+        <v>44</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" t="s">
-        <v>51</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" si="0"/>
-        <v>ISLDFN</v>
+      <c r="I11" t="s">
+        <v>19</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" t="s">
         <v>11</v>
       </c>
-      <c r="H12" t="s">
-        <v>53</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" si="0"/>
-        <v>ISLDDC</v>
+      <c r="I12" t="s">
+        <v>46</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
         <v>11</v>
       </c>
-      <c r="H13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" si="0"/>
-        <v>SESTRG</v>
+      <c r="I13" t="s">
+        <v>48</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
         <v>11</v>
       </c>
-      <c r="H14" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="0"/>
-        <v>CULUSA</v>
+      <c r="I14" t="s">
+        <v>52</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M15" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M16" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M17" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M18" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M19" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M20" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M21" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M22" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M23" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M24" t="e">
-        <f t="shared" ref="M24" si="2">+MID(F24,8,LEN(F24)-7)</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="N24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M25" t="e">
-        <f t="shared" ref="M25:M29" si="3">+MID(F25,8,LEN(F25)-7)</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="N25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M26" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M27" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="N27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M28" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="M28" t="str">
+        <f t="shared" ref="M3:M32" si="1">+MID(F28,1,LEN(F28))</f>
+        <v/>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M29" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+      <c r="M29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M32" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +1773,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>N2:N29</xm:sqref>
+          <xm:sqref>N2:N30</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Actualizacion de scripts de prorrogas, se verifican los mensajes de salida segun especificacion del documento
</commit_message>
<xml_diff>
--- a/Otros (Plantillas, etc)/plantilla codigo.xlsx
+++ b/Otros (Plantillas, etc)/plantilla codigo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>IN PARAM_CCMPN</t>
   </si>
@@ -27,9 +27,6 @@
     <t>CHAR (1),</t>
   </si>
   <si>
-    <t>IN PARAM_NPROPR</t>
-  </si>
-  <si>
     <t>NUMERIC (10, 0),</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>:</t>
   </si>
   <si>
-    <t>Código de compañía – Alfanumérico (2)</t>
-  </si>
-  <si>
     <t>Match</t>
   </si>
   <si>
@@ -66,142 +60,178 @@
     <t>Parametro documento</t>
   </si>
   <si>
-    <t>IN PARAM_CRGMN</t>
-  </si>
-  <si>
     <t>CHAR (1) ,</t>
   </si>
   <si>
-    <t>Numero de Pre-Operación  - Numérico (10, 0)</t>
-  </si>
-  <si>
-    <t>Código usuario actualizador – Alfanumérico (10)</t>
-  </si>
-  <si>
-    <t>IN PARAM_CTPOAL</t>
-  </si>
-  <si>
-    <t>IN PARAM_CFNNC</t>
-  </si>
-  <si>
-    <t>IN PARAM_CSCRS</t>
-  </si>
-  <si>
-    <t>IN PARAM_CALMCM</t>
-  </si>
-  <si>
-    <t>IN PARAM_CMNDA</t>
-  </si>
-  <si>
-    <t>IN PARAM_SIMPR</t>
-  </si>
-  <si>
-    <t>IN PARAM_CADNA</t>
-  </si>
-  <si>
-    <t>IN PARAM_NANDCL</t>
-  </si>
-  <si>
-    <t>IN PARAM_NPDDUA</t>
-  </si>
-  <si>
     <t>CCMPN</t>
   </si>
   <si>
-    <t>NPROPR</t>
-  </si>
-  <si>
-    <t>CTPOAL</t>
-  </si>
-  <si>
-    <t>Código tipo almacén – Alfanumérico (1)</t>
-  </si>
-  <si>
-    <t>CFNNC</t>
-  </si>
-  <si>
-    <t>Código de Financiador – Numérico (4,0)</t>
-  </si>
-  <si>
-    <t>CSCRS</t>
-  </si>
-  <si>
-    <t>Código de sucursal -  Numérico (4,0)</t>
-  </si>
-  <si>
-    <t>CALMCM</t>
-  </si>
-  <si>
-    <t>Código de Almacén – Numérico (6,0)</t>
-  </si>
-  <si>
-    <t>CMNDA</t>
-  </si>
-  <si>
-    <t>Código de moneda – Numérico (3,0)</t>
-  </si>
-  <si>
-    <t>CRGMN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código de régimen – Alfanumérico (1) </t>
-  </si>
-  <si>
-    <t>SIMPR</t>
-  </si>
-  <si>
-    <t>Flag impresión – Alfanumérico (1)</t>
-  </si>
-  <si>
-    <t>CADNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código de Aduana – Numérico (6,0)  </t>
-  </si>
-  <si>
-    <t>NANDCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Año declaración DUA – Numérico (4,0)  </t>
-  </si>
-  <si>
-    <t>NPDDUA</t>
-  </si>
-  <si>
-    <t>CHAR (2) ,</t>
-  </si>
-  <si>
     <t>NUMERIC (6,0) ,</t>
   </si>
   <si>
-    <t xml:space="preserve">Número pedido. depósito DUA– Numérico (10,0) </t>
-  </si>
-  <si>
-    <t>NUMERIC (6,0)   ,</t>
-  </si>
-  <si>
-    <t>NUMERIC (4,0)   ,</t>
-  </si>
-  <si>
-    <t>NUMERIC (10,0)   ,</t>
-  </si>
-  <si>
     <t>CULUSA</t>
   </si>
   <si>
-    <t>NUMERIC (10, 0) ,</t>
-  </si>
-  <si>
-    <t>NUMERIC (3,0) ,</t>
-  </si>
-  <si>
-    <t>NUMERIC (4,0) ,</t>
-  </si>
-  <si>
-    <t>CHAR (1)  ,</t>
-  </si>
-  <si>
-    <t>CHAR (10) ,</t>
+    <t>IN PARAM_NOPRCN</t>
+  </si>
+  <si>
+    <t>IN PARAM_NWRRNT</t>
+  </si>
+  <si>
+    <t>IN PARAM_CCLNT</t>
+  </si>
+  <si>
+    <t>NUMERIC (6,0),</t>
+  </si>
+  <si>
+    <t>IN PARAM_CBNCFN</t>
+  </si>
+  <si>
+    <t>NUMERIC (4,0),</t>
+  </si>
+  <si>
+    <t>IN PARAM_NFRMAL</t>
+  </si>
+  <si>
+    <t>NUMERIC (2,0 ),</t>
+  </si>
+  <si>
+    <t>IN PARAM_NENDS</t>
+  </si>
+  <si>
+    <t>IN PARAM_SFRMAL</t>
+  </si>
+  <si>
+    <t>IN PARAM_SFRMBN</t>
+  </si>
+  <si>
+    <t>IN PARAM_SFRMCL</t>
+  </si>
+  <si>
+    <t>IN PARAM_NFRRAL</t>
+  </si>
+  <si>
+    <t>NUMERIC (2,0),</t>
+  </si>
+  <si>
+    <t>IN PARAM_NFRRBN</t>
+  </si>
+  <si>
+    <t>IN PARAM_NFRMBN</t>
+  </si>
+  <si>
+    <t>IN PARAM_NFRRCL</t>
+  </si>
+  <si>
+    <t>IN PARAM_NFRMCL</t>
+  </si>
+  <si>
+    <t>Código Compañía – Alfanumérico (2)</t>
+  </si>
+  <si>
+    <t>NSLCPR</t>
+  </si>
+  <si>
+    <t>Numero Solicitud Prórroga - Numérico (10, 0)</t>
+  </si>
+  <si>
+    <t>NOPRCN</t>
+  </si>
+  <si>
+    <t>Numero de Operación  - Numérico (10, 0)</t>
+  </si>
+  <si>
+    <t>NWRRNT</t>
+  </si>
+  <si>
+    <t>Numero de Warrant  - Numérico (10, 0)</t>
+  </si>
+  <si>
+    <t>CCLNT</t>
+  </si>
+  <si>
+    <t>Código de Cliente – Numérico (6,0)</t>
+  </si>
+  <si>
+    <t>CBNCFN</t>
+  </si>
+  <si>
+    <t>Código del  Banco – Financiera – Numérico (4,0)</t>
+  </si>
+  <si>
+    <t>NFRMAL</t>
+  </si>
+  <si>
+    <t>Numero Firmas de Almacenera – Numérico (2,0 )</t>
+  </si>
+  <si>
+    <t>SESTRG</t>
+  </si>
+  <si>
+    <t>Flag Estado del Registro – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>CódIgo Ultimo Usuario Actualizador – Alfanumérico (10)</t>
+  </si>
+  <si>
+    <t>NTRMNL</t>
+  </si>
+  <si>
+    <t>Número de Terminal Usado– Alfanumérico  (10)</t>
+  </si>
+  <si>
+    <t>NENDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numero de Endoso – Numérico (10,0) </t>
+  </si>
+  <si>
+    <t>SFRMAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag Firma de Almacenera - Alfanumérico (1) </t>
+  </si>
+  <si>
+    <t>SFRMBN</t>
+  </si>
+  <si>
+    <t>Flag Firma del Banco - Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>SFRMCL</t>
+  </si>
+  <si>
+    <t>Flag Firma del cliente - Alfanumérico (1).</t>
+  </si>
+  <si>
+    <t>NFRRAL</t>
+  </si>
+  <si>
+    <t>Numero Firmas Registradas Almacenera – Numérico (2,0)</t>
+  </si>
+  <si>
+    <t>NFRRBN</t>
+  </si>
+  <si>
+    <t>Numero Firmas Registradas del banco – Numérico (2,0)</t>
+  </si>
+  <si>
+    <t>NFRMBN</t>
+  </si>
+  <si>
+    <t>Numero Firmas del Banco – Numérico (2,0)</t>
+  </si>
+  <si>
+    <t>NFRRCL</t>
+  </si>
+  <si>
+    <t>Numero Firmas Registradas del Cliente – Numérico (2,0)</t>
+  </si>
+  <si>
+    <t>NFRMCL</t>
+  </si>
+  <si>
+    <t>Numero Firmas del Cliente – Numérico (2,0)</t>
   </si>
 </sst>
 </file>
@@ -615,10 +645,10 @@
         <v>IN PARAM_NSLCPR NUMERIC (10, 0),</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F26" si="1">+MID(A2,4,LEN(A2)-2)</f>
@@ -647,7 +677,7 @@
         <v>IN PARAM_SESTRG CHAR (1),</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -679,10 +709,10 @@
         <v>IN PARAM_CULUSA CHAR (10),</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -711,10 +741,10 @@
         <v>IN PARAM_NTRMNL CHAR  (10),</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1257,7 +1287,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A14"/>
+      <selection activeCell="F2" sqref="F2:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,13 +1300,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1287,19 +1317,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1">
         <f>IF(ISERROR(FIND(F2,A2,1)),0,IF(ISBLANK(F2),0,1))</f>
@@ -1308,25 +1335,22 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N30" si="0">IF(ISERROR(FIND(F3,A3,1)),0,IF(ISBLANK(F3),0,1))</f>
@@ -1335,25 +1359,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" si="0"/>
@@ -1362,25 +1383,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
@@ -1389,25 +1407,22 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
@@ -1416,25 +1431,22 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
@@ -1443,25 +1455,22 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
@@ -1470,25 +1479,22 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
@@ -1497,25 +1503,22 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
@@ -1524,25 +1527,22 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
@@ -1557,19 +1557,16 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="0"/>
@@ -1584,19 +1581,16 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="0"/>
@@ -1611,19 +1605,16 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="0"/>
@@ -1631,120 +1622,228 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>61</v>
+      </c>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>63</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" t="s">
+        <v>71</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N21" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N16" s="1">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N22" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N17" s="1">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N18" s="1">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N24" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N19" s="1">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N25" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N20" s="1">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N26" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N21" s="1">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N27" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N22" s="1">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M28" t="str">
+        <f t="shared" ref="M28:M32" si="1">+MID(F28,1,LEN(F28))</f>
+        <v/>
+      </c>
+      <c r="N28" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N23" s="1">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N29" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N24" s="1">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="N30" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N25" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N26" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N27" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M28" t="str">
-        <f t="shared" ref="M3:M32" si="1">+MID(F28,1,LEN(F28))</f>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M31" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N28" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M29" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N29" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="N30" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M31" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="13:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M32" t="str">
         <f t="shared" si="1"/>
         <v/>

</xml_diff>

<commit_message>
Actualizacion de script de Generales por cambio en documento funcional, se adiciona ultima version del documento de generales
</commit_message>
<xml_diff>
--- a/Otros (Plantillas, etc)/plantilla codigo.xlsx
+++ b/Otros (Plantillas, etc)/plantilla codigo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>IN PARAM_CCMPN</t>
   </si>
@@ -66,172 +66,103 @@
     <t>CCMPN</t>
   </si>
   <si>
-    <t>NUMERIC (6,0) ,</t>
-  </si>
-  <si>
     <t>CULUSA</t>
   </si>
   <si>
     <t>IN PARAM_NOPRCN</t>
   </si>
   <si>
-    <t>IN PARAM_NWRRNT</t>
-  </si>
-  <si>
-    <t>IN PARAM_CCLNT</t>
-  </si>
-  <si>
     <t>NUMERIC (6,0),</t>
   </si>
   <si>
-    <t>IN PARAM_CBNCFN</t>
-  </si>
-  <si>
-    <t>NUMERIC (4,0),</t>
-  </si>
-  <si>
-    <t>IN PARAM_NFRMAL</t>
-  </si>
-  <si>
-    <t>NUMERIC (2,0 ),</t>
-  </si>
-  <si>
-    <t>IN PARAM_NENDS</t>
-  </si>
-  <si>
-    <t>IN PARAM_SFRMAL</t>
-  </si>
-  <si>
-    <t>IN PARAM_SFRMBN</t>
-  </si>
-  <si>
-    <t>IN PARAM_SFRMCL</t>
-  </si>
-  <si>
-    <t>IN PARAM_NFRRAL</t>
-  </si>
-  <si>
-    <t>NUMERIC (2,0),</t>
-  </si>
-  <si>
-    <t>IN PARAM_NFRRBN</t>
-  </si>
-  <si>
-    <t>IN PARAM_NFRMBN</t>
-  </si>
-  <si>
-    <t>IN PARAM_NFRRCL</t>
-  </si>
-  <si>
-    <t>IN PARAM_NFRMCL</t>
-  </si>
-  <si>
-    <t>Código Compañía – Alfanumérico (2)</t>
-  </si>
-  <si>
-    <t>NSLCPR</t>
-  </si>
-  <si>
-    <t>Numero Solicitud Prórroga - Numérico (10, 0)</t>
-  </si>
-  <si>
     <t>NOPRCN</t>
   </si>
   <si>
-    <t>Numero de Operación  - Numérico (10, 0)</t>
-  </si>
-  <si>
-    <t>NWRRNT</t>
-  </si>
-  <si>
-    <t>Numero de Warrant  - Numérico (10, 0)</t>
-  </si>
-  <si>
-    <t>CCLNT</t>
-  </si>
-  <si>
-    <t>Código de Cliente – Numérico (6,0)</t>
-  </si>
-  <si>
-    <t>CBNCFN</t>
-  </si>
-  <si>
-    <t>Código del  Banco – Financiera – Numérico (4,0)</t>
-  </si>
-  <si>
-    <t>NFRMAL</t>
-  </si>
-  <si>
-    <t>Numero Firmas de Almacenera – Numérico (2,0 )</t>
-  </si>
-  <si>
     <t>SESTRG</t>
   </si>
   <si>
-    <t>Flag Estado del Registro – Alfanumérico (1)</t>
-  </si>
-  <si>
-    <t>CódIgo Ultimo Usuario Actualizador – Alfanumérico (10)</t>
-  </si>
-  <si>
-    <t>NTRMNL</t>
-  </si>
-  <si>
-    <t>Número de Terminal Usado– Alfanumérico  (10)</t>
-  </si>
-  <si>
-    <t>NENDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numero de Endoso – Numérico (10,0) </t>
-  </si>
-  <si>
-    <t>SFRMAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flag Firma de Almacenera - Alfanumérico (1) </t>
-  </si>
-  <si>
-    <t>SFRMBN</t>
-  </si>
-  <si>
-    <t>Flag Firma del Banco - Alfanumérico (1)</t>
-  </si>
-  <si>
-    <t>SFRMCL</t>
-  </si>
-  <si>
-    <t>Flag Firma del cliente - Alfanumérico (1).</t>
-  </si>
-  <si>
-    <t>NFRRAL</t>
-  </si>
-  <si>
-    <t>Numero Firmas Registradas Almacenera – Numérico (2,0)</t>
-  </si>
-  <si>
-    <t>NFRRBN</t>
-  </si>
-  <si>
-    <t>Numero Firmas Registradas del banco – Numérico (2,0)</t>
-  </si>
-  <si>
-    <t>NFRMBN</t>
-  </si>
-  <si>
-    <t>Numero Firmas del Banco – Numérico (2,0)</t>
-  </si>
-  <si>
-    <t>NFRRCL</t>
-  </si>
-  <si>
-    <t>Numero Firmas Registradas del Cliente – Numérico (2,0)</t>
-  </si>
-  <si>
-    <t>NFRMCL</t>
-  </si>
-  <si>
-    <t>Numero Firmas del Cliente – Numérico (2,0)</t>
+    <t>IN PARAM_NPROPR</t>
+  </si>
+  <si>
+    <t>Código de compañía – Alfanumérico (2)</t>
+  </si>
+  <si>
+    <t>NPROPR</t>
+  </si>
+  <si>
+    <t>Numero de Pre-Operación  - Numérico (10, 0)</t>
+  </si>
+  <si>
+    <t>Código usuario actualizador – Alfanumérico (10)</t>
+  </si>
+  <si>
+    <t>NUMERIC (5,0),</t>
+  </si>
+  <si>
+    <t>Numero de Item – Numérico (5,0)</t>
+  </si>
+  <si>
+    <t>NUMERIC (8,0),</t>
+  </si>
+  <si>
+    <t>IN PARAM_STPENT</t>
+  </si>
+  <si>
+    <t>IN PARAM_CENTD</t>
+  </si>
+  <si>
+    <t>IN PARAM_CRPRS</t>
+  </si>
+  <si>
+    <t>CHAR (5),</t>
+  </si>
+  <si>
+    <t>IN PARAM_SFRMRP</t>
+  </si>
+  <si>
+    <t>IN PARAM_FFRMRP</t>
+  </si>
+  <si>
+    <t>IN PARAM_HFRMRP</t>
+  </si>
+  <si>
+    <t>STPENT</t>
+  </si>
+  <si>
+    <t>CENTD</t>
+  </si>
+  <si>
+    <t>Código de entidad – Numérico (6,0)</t>
+  </si>
+  <si>
+    <t>CRPRS</t>
+  </si>
+  <si>
+    <t>Código representante – Alfanumérico (5)</t>
+  </si>
+  <si>
+    <t>Número Operación – Numérico (10, 0)</t>
+  </si>
+  <si>
+    <t>SFRMRP</t>
+  </si>
+  <si>
+    <t>Flag firma del representante – Alfanumérico (1)</t>
+  </si>
+  <si>
+    <t>FFRMRP</t>
+  </si>
+  <si>
+    <t>Fecha firma representante – Numérico (8,0)</t>
+  </si>
+  <si>
+    <t>HFRMRP</t>
+  </si>
+  <si>
+    <t>Hora firma representante – Numérico (6,0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flag estado registro – Alfanumérico (1) </t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1218,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H20"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1257,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="N2" s="1">
         <f>IF(ISERROR(FIND(F2,A2,1)),0,IF(ISBLANK(F2),0,1))</f>
@@ -1335,22 +1266,22 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N30" si="0">IF(ISERROR(FIND(F3,A3,1)),0,IF(ISBLANK(F3),0,1))</f>
@@ -1359,22 +1290,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" si="0"/>
@@ -1383,22 +1314,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
@@ -1407,22 +1338,22 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
@@ -1431,22 +1362,22 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
@@ -1455,22 +1386,22 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
@@ -1479,22 +1410,22 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
@@ -1503,22 +1434,22 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
@@ -1527,22 +1458,22 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
@@ -1551,22 +1482,22 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="0"/>
@@ -1574,240 +1505,96 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" t="s">
-        <v>57</v>
-      </c>
       <c r="N13" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" t="s">
-        <v>59</v>
-      </c>
       <c r="N14" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" t="s">
-        <v>61</v>
-      </c>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" t="s">
-        <v>63</v>
-      </c>
       <c r="N16" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N17" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" t="s">
-        <v>67</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N18" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" t="s">
-        <v>69</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N19" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" t="s">
-        <v>71</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N20" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N21" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N22" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N23" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N24" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N25" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N26" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="13:14" x14ac:dyDescent="0.25">
       <c r="N27" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M28" t="str">
         <f t="shared" ref="M28:M32" si="1">+MID(F28,1,LEN(F28))</f>
         <v/>
@@ -1817,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M29" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1827,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M30" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1837,13 +1624,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M32" t="str">
         <f t="shared" si="1"/>
         <v/>

</xml_diff>

<commit_message>
Actualizacion de documentacion funcional WARRANTS, LIBERACIONES, ajustes a procedimientos almacenados
</commit_message>
<xml_diff>
--- a/Otros (Plantillas, etc)/plantilla codigo.xlsx
+++ b/Otros (Plantillas, etc)/plantilla codigo.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9975" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Generador Parametros" sheetId="1" r:id="rId1"/>
     <sheet name="Comparador Parametros" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Test procedures" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>IN PARAM_CCMPN</t>
   </si>
@@ -163,6 +163,48 @@
   </si>
   <si>
     <t xml:space="preserve">Flag estado registro – Alfanumérico (1) </t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>IN PARAM_CCMPN CHAR(2),</t>
+  </si>
+  <si>
+    <t>INOUT PARAM_PROCSTATUS INT,</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>IN PARAM_STPENT CHAR (1),</t>
+  </si>
+  <si>
+    <t>IN PARAM_CENTD NUMERIC (6, 0),</t>
+  </si>
+  <si>
+    <t>IN PARAM_CRPRS CHAR (5),</t>
+  </si>
+  <si>
+    <t>IN PARAM_TRPRS CHAR (30),</t>
+  </si>
+  <si>
+    <t>IN PARAM_TRUTFR CHAR (50),</t>
+  </si>
+  <si>
+    <t>IN PARAM_TDRCRD CHAR (50),</t>
+  </si>
+  <si>
+    <t>IN PARAM_SESTRG CHAR (1),</t>
+  </si>
+  <si>
+    <t>IN PARAM_CULUSA CHAR (10),</t>
+  </si>
+  <si>
+    <t>CREATE PROCEDURE INTEGRASGO.SP_INTSGO_GEN_ACTUALIZA_REPRESENTANTE</t>
+  </si>
+  <si>
+    <t>INOUT PARAM_PROCDESC VARCHAR(2000)</t>
   </si>
 </sst>
 </file>
@@ -962,7 +1004,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="shared" ref="A17:A18" si="6">+CONCATENATE(B17," ",C17)</f>
+        <f>+CONCATENATE(B17," ",C17)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F17" t="e">
@@ -988,7 +1030,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="6"/>
+        <f>+CONCATENATE(B18," ",C18)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F18" t="e">
@@ -1146,7 +1188,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" ref="A25:A27" si="7">+CONCATENATE(B25," ",C25)</f>
+        <f>+CONCATENATE(B25," ",C25)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F25" t="e">
@@ -1172,7 +1214,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" si="7"/>
+        <f>+CONCATENATE(B26," ",C26)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F26" t="e">
@@ -1198,7 +1240,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="7"/>
+        <f>+CONCATENATE(B27," ",C27)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1217,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -1596,7 +1638,7 @@
     </row>
     <row r="28" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M28" t="str">
-        <f t="shared" ref="M28:M32" si="1">+MID(F28,1,LEN(F28))</f>
+        <f>+MID(F28,1,LEN(F28))</f>
         <v/>
       </c>
       <c r="N28" s="1">
@@ -1606,7 +1648,7 @@
     </row>
     <row r="29" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M29" t="str">
-        <f t="shared" si="1"/>
+        <f>+MID(F29,1,LEN(F29))</f>
         <v/>
       </c>
       <c r="N29" s="1">
@@ -1616,7 +1658,7 @@
     </row>
     <row r="30" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M30" t="str">
-        <f t="shared" si="1"/>
+        <f>+MID(F30,1,LEN(F30))</f>
         <v/>
       </c>
       <c r="N30" s="1">
@@ -1626,13 +1668,13 @@
     </row>
     <row r="31" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M31" t="str">
-        <f t="shared" si="1"/>
+        <f>+MID(F31,1,LEN(F31))</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M32" t="str">
-        <f t="shared" si="1"/>
+        <f>+MID(F32,1,LEN(F32))</f>
         <v/>
       </c>
     </row>
@@ -1669,12 +1711,183 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="10" max="10" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1">
+        <v>16</v>
+      </c>
+      <c r="J1" t="str">
+        <f>+MID(A1,18,LEN(A1)-16)</f>
+        <v>INTEGRASGO.SP_INTSGO_GEN_ACTUALIZA_REPRESENTANTE</v>
+      </c>
+      <c r="K1" t="str">
+        <f>+CONCATENATE("CALL ",J1)</f>
+        <v>CALL INTEGRASGO.SP_INTSGO_GEN_ACTUALIZA_REPRESENTANTE</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="str">
+        <f>+A2</f>
+        <v>(</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" t="str">
+        <f>CONCATENATE(IF(NOT(ISERROR(FIND("CHAR",A3,1))),"''",IF(NOT(ISERROR(FIND("NUMERIC",A3,1))),"0","*")),",","--",A3)</f>
+        <v>'',--IN PARAM_CCMPN CHAR(2),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:L13" si="0">CONCATENATE(IF(NOT(ISERROR(FIND("CHAR",A4,1))),"''",IF(NOT(ISERROR(FIND("NUMERIC",A4,1))),"0","*")),",","--",A4)</f>
+        <v>'',--IN PARAM_STPENT CHAR (1),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>0,--IN PARAM_CENTD NUMERIC (6, 0),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>'',--IN PARAM_CRPRS CHAR (5),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>'',--IN PARAM_TRPRS CHAR (30),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>'',--IN PARAM_TRUTFR CHAR (50),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>'',--IN PARAM_TDRCRD CHAR (50),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>'',--IN PARAM_SESTRG CHAR (1),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>'',--IN PARAM_CULUSA CHAR (10),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>*,--INOUT PARAM_PROCSTATUS INT,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>'',--INOUT PARAM_PROCDESC VARCHAR(2000)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" ref="L14:L19" si="1">CONCATENATE(IF(NOT(ISERROR(FIND("CHAR",A14,1))),"''",IF(NOT(ISERROR(FIND("NUMERIC",A14,1))),"0","*")),",","--",A14)</f>
+        <v>*,--)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" t="str">
+        <f t="shared" si="1"/>
+        <v>*,--</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" t="str">
+        <f t="shared" si="1"/>
+        <v>*,--</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" t="str">
+        <f t="shared" si="1"/>
+        <v>*,--</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="str">
+        <f t="shared" si="1"/>
+        <v>*,--</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19" t="str">
+        <f t="shared" si="1"/>
+        <v>*,--</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="120" verticalDpi="72" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>